<commit_message>
Updated dates in K Joyce Mohamed collection
</commit_message>
<xml_diff>
--- a/Photographic Archive/K JOYCE MOHAMED.xlsx
+++ b/Photographic Archive/K JOYCE MOHAMED.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Z$1</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -4701,6 +4704,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Z1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removed acquisition date from K Joyce Mohamed collection
</commit_message>
<xml_diff>
--- a/Photographic Archive/K JOYCE MOHAMED.xlsx
+++ b/Photographic Archive/K JOYCE MOHAMED.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="332">
   <si>
     <t>identifier</t>
   </si>
@@ -43,24 +43,9 @@
     <t>file_path</t>
   </si>
   <si>
-    <t>ACCESSION NO</t>
-  </si>
-  <si>
-    <t>TITLE</t>
-  </si>
-  <si>
-    <t>ACQUISITION NO.</t>
-  </si>
-  <si>
     <t>Item</t>
   </si>
   <si>
-    <t>ITEM DESCRIPTION</t>
-  </si>
-  <si>
-    <t>LOCATION | SECTION</t>
-  </si>
-  <si>
     <t>QTY</t>
   </si>
   <si>
@@ -77,9 +62,6 @@
   </si>
   <si>
     <t>PICTURE MOHAMED, K JOYCE</t>
-  </si>
-  <si>
-    <t>01/04/2014</t>
   </si>
   <si>
     <t>PICTURE</t>
@@ -1313,11 +1295,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z105"/>
+  <dimension ref="A1:Z104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1327,8 +1309,9 @@
     <col min="5" max="5" width="15.109375" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" customWidth="1"/>
     <col min="7" max="7" width="39.44140625" customWidth="1"/>
-    <col min="8" max="9" width="92.33203125" customWidth="1"/>
-    <col min="11" max="14" width="0" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" customWidth="1"/>
+    <col min="11" max="14" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1358,10 +1341,18 @@
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
@@ -1377,3330 +1368,3055 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>10</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D2" s="5"/>
       <c r="E2" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="M2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="N2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D3" s="5"/>
       <c r="E3" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
         <v>22</v>
       </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>23</v>
       </c>
-      <c r="M3" t="s">
-        <v>24</v>
-      </c>
       <c r="N3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="M4" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M4" t="s">
-        <v>29</v>
-      </c>
       <c r="N4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M5" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5" t="s">
-        <v>32</v>
-      </c>
-      <c r="M5" t="s">
-        <v>33</v>
-      </c>
       <c r="N5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D6" s="5"/>
       <c r="E6" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K6">
         <v>1</v>
       </c>
       <c r="L6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="M6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="N6" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D7" s="5"/>
       <c r="E7" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K7">
         <v>1</v>
       </c>
       <c r="L7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="M7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="N7" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8" t="s">
+        <v>39</v>
+      </c>
+      <c r="M8" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
-      <c r="L8" t="s">
-        <v>41</v>
-      </c>
-      <c r="M8" t="s">
-        <v>42</v>
-      </c>
       <c r="N8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9" t="s">
+        <v>42</v>
+      </c>
+      <c r="M9" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K9">
-        <v>1</v>
-      </c>
-      <c r="L9" t="s">
-        <v>45</v>
-      </c>
-      <c r="M9" t="s">
-        <v>46</v>
-      </c>
       <c r="N9" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D10" s="5"/>
       <c r="E10" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K10">
         <v>1</v>
       </c>
       <c r="L10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="M10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="N10" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D11" s="5"/>
       <c r="E11" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K11">
         <v>1</v>
       </c>
       <c r="L11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="M11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="N11" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D12" s="5"/>
       <c r="E12" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K12">
         <v>1</v>
       </c>
       <c r="L12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="M12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="N12" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D13" s="5"/>
       <c r="E13" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K13">
         <v>1</v>
       </c>
       <c r="L13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="M13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="N13" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D14" s="5"/>
       <c r="E14" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K14">
         <v>1</v>
       </c>
       <c r="L14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="M14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="N14" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D15" s="5"/>
       <c r="E15" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K15">
         <v>1</v>
       </c>
       <c r="L15" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="M15" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="N15" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D16" s="5"/>
       <c r="E16" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K16">
         <v>1</v>
       </c>
       <c r="L16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="N16" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D17" s="5"/>
       <c r="E17" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K17">
         <v>1</v>
       </c>
       <c r="L17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="N17" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D18" s="5"/>
       <c r="E18" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K18">
         <v>1</v>
       </c>
       <c r="L18" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="M18" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="N18" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19" t="s">
+        <v>73</v>
+      </c>
+      <c r="M19" t="s">
         <v>74</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K19">
-        <v>1</v>
-      </c>
-      <c r="L19" t="s">
-        <v>75</v>
-      </c>
-      <c r="M19" t="s">
-        <v>76</v>
-      </c>
       <c r="N19" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20" t="s">
+        <v>76</v>
+      </c>
+      <c r="M20" t="s">
         <v>77</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K20">
-        <v>1</v>
-      </c>
-      <c r="L20" t="s">
-        <v>79</v>
-      </c>
-      <c r="M20" t="s">
-        <v>80</v>
-      </c>
       <c r="N20" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D21" s="5"/>
       <c r="E21" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K21">
         <v>1</v>
       </c>
       <c r="L21" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="M21" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="N21" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D22" s="5"/>
       <c r="E22" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K22">
         <v>1</v>
       </c>
       <c r="L22" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="M22" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="N22" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D23" s="5"/>
       <c r="E23" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K23">
         <v>1</v>
       </c>
       <c r="L23" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="M23" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="N23" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D24" s="5"/>
       <c r="E24" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K24">
         <v>1</v>
       </c>
       <c r="L24" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="M24" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="N24" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D25" s="5"/>
       <c r="E25" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K25">
         <v>1</v>
       </c>
       <c r="L25" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="M25" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="N25" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="5"/>
+      <c r="E26" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26" t="s">
+        <v>94</v>
+      </c>
+      <c r="M26" t="s">
+        <v>95</v>
+      </c>
+      <c r="N26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K26">
-        <v>1</v>
-      </c>
-      <c r="L26" t="s">
+      <c r="C27" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="5"/>
+      <c r="E27" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27" t="s">
         <v>97</v>
       </c>
-      <c r="M26" t="s">
+      <c r="M27" t="s">
         <v>98</v>
       </c>
-      <c r="N26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K27">
-        <v>1</v>
-      </c>
-      <c r="L27" t="s">
-        <v>100</v>
-      </c>
-      <c r="M27" t="s">
-        <v>101</v>
-      </c>
       <c r="N27" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D28" s="5"/>
       <c r="E28" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K28">
         <v>1</v>
       </c>
       <c r="L28" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="M28" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="N28" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D29" s="5"/>
       <c r="E29" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K29">
         <v>1</v>
       </c>
       <c r="L29" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="M29" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="N29" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D30" s="5"/>
+      <c r="E30" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30" t="s">
+        <v>107</v>
+      </c>
+      <c r="M30" t="s">
         <v>108</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K30">
-        <v>1</v>
-      </c>
-      <c r="L30" t="s">
-        <v>109</v>
-      </c>
-      <c r="M30" t="s">
-        <v>110</v>
-      </c>
       <c r="N30" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+      <c r="L31" t="s">
+        <v>110</v>
+      </c>
+      <c r="M31" t="s">
         <v>111</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K31">
-        <v>1</v>
-      </c>
-      <c r="L31" t="s">
-        <v>113</v>
-      </c>
-      <c r="M31" t="s">
-        <v>114</v>
-      </c>
       <c r="N31" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D32" s="5"/>
       <c r="E32" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K32">
         <v>1</v>
       </c>
       <c r="L32" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="M32" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="N32" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D33" s="5"/>
       <c r="E33" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K33">
         <v>1</v>
       </c>
       <c r="L33" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M33" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="N33" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D34" s="5"/>
       <c r="E34" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K34">
         <v>1</v>
       </c>
       <c r="L34" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M34" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="N34" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D35" s="5"/>
       <c r="E35" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K35">
         <v>1</v>
       </c>
       <c r="L35" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="M35" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="N35" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D36" s="5"/>
       <c r="E36" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K36">
         <v>1</v>
       </c>
       <c r="L36" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="M36" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="N36" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D37" s="5"/>
       <c r="E37" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K37">
         <v>1</v>
       </c>
       <c r="L37" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="M37" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="N37" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D38" s="5"/>
       <c r="E38" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K38">
         <v>1</v>
       </c>
       <c r="L38" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M38" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="N38" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D39" s="5"/>
       <c r="E39" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K39">
         <v>1</v>
       </c>
       <c r="L39" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="M39" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="N39" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D40" s="5"/>
       <c r="E40" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K40">
         <v>1</v>
       </c>
       <c r="L40" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="M40" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="N40" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D41" s="5"/>
       <c r="E41" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K41">
         <v>1</v>
       </c>
       <c r="L41" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="M41" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="N41" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D42" s="5"/>
       <c r="E42" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K42">
         <v>1</v>
       </c>
       <c r="L42" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="M42" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="N42" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D43" s="5"/>
       <c r="E43" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K43">
         <v>1</v>
       </c>
       <c r="L43" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="M43" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="N43" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D44" s="5"/>
       <c r="E44" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K44">
         <v>1</v>
       </c>
       <c r="L44" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="M44" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="N44" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D45" s="5"/>
       <c r="E45" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K45">
         <v>1</v>
       </c>
       <c r="L45" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="M45" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="N45" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D46" s="5"/>
       <c r="E46" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K46">
         <v>1</v>
       </c>
       <c r="L46" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="M46" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="N46" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D47" s="5"/>
       <c r="E47" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K47">
         <v>1</v>
       </c>
       <c r="L47" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="M47" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="N47" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D48" s="5"/>
       <c r="E48" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K48">
         <v>1</v>
       </c>
       <c r="L48" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="M48" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="N48" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="49" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D49" s="5"/>
       <c r="E49" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K49">
         <v>1</v>
       </c>
       <c r="L49" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="M49" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="N49" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="50" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D50" s="5"/>
       <c r="E50" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K50">
         <v>1</v>
       </c>
       <c r="L50" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="M50" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="N50" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="51" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D51" s="5"/>
       <c r="E51" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K51">
         <v>1</v>
       </c>
       <c r="L51" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="M51" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="N51" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="52" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D52" s="5"/>
       <c r="E52" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K52">
         <v>1</v>
       </c>
       <c r="L52" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="M52" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="N52" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="53" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D53" s="5"/>
       <c r="E53" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K53">
         <v>1</v>
       </c>
       <c r="L53" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="M53" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="N53" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="54" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D54" s="5"/>
       <c r="E54" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K54">
         <v>1</v>
       </c>
       <c r="L54" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="M54" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="N54" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="55" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D55" s="5"/>
       <c r="E55" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K55">
         <v>1</v>
       </c>
       <c r="L55" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="M55" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="N55" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="56" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D56" s="5"/>
       <c r="E56" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K56">
         <v>1</v>
       </c>
       <c r="L56" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="M56" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="N56" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="57" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D57" s="5"/>
       <c r="E57" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K57">
         <v>1</v>
       </c>
       <c r="L57" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="M57" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="N57" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="58" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D58" s="5"/>
       <c r="E58" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K58">
         <v>1</v>
       </c>
       <c r="L58" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="M58" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="N58" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="59" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D59" s="5"/>
       <c r="E59" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K59">
         <v>1</v>
       </c>
       <c r="L59" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="M59" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="N59" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="60" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D60" s="5"/>
       <c r="E60" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K60">
         <v>1</v>
       </c>
       <c r="L60" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="M60" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="N60" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="61" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D61" s="5"/>
       <c r="E61" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K61">
         <v>1</v>
       </c>
       <c r="L61" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="M61" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="N61" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="62" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D62" s="5"/>
       <c r="E62" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K62">
         <v>1</v>
       </c>
       <c r="L62" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="M62" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="N62" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="63" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D63" s="5"/>
       <c r="E63" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F63" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K63">
         <v>1</v>
       </c>
       <c r="L63" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="M63" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="N63" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="64" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D64" s="5"/>
       <c r="E64" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K64">
         <v>1</v>
       </c>
       <c r="L64" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M64" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="N64" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="65" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D65" s="5"/>
+      <c r="E65" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G65" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="K65">
+        <v>1</v>
+      </c>
+      <c r="L65" t="s">
+        <v>213</v>
+      </c>
+      <c r="M65" t="s">
         <v>214</v>
       </c>
-      <c r="C65" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E65" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F65" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G65" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K65">
-        <v>1</v>
-      </c>
-      <c r="L65" t="s">
-        <v>215</v>
-      </c>
-      <c r="M65" t="s">
-        <v>216</v>
-      </c>
       <c r="N65" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="66" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D66" s="5"/>
+      <c r="E66" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="K66">
+        <v>1</v>
+      </c>
+      <c r="L66" t="s">
+        <v>216</v>
+      </c>
+      <c r="M66" t="s">
         <v>217</v>
       </c>
-      <c r="C66" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F66" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G66" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="K66">
-        <v>1</v>
-      </c>
-      <c r="L66" t="s">
-        <v>219</v>
-      </c>
-      <c r="M66" t="s">
-        <v>220</v>
-      </c>
       <c r="N66" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="67" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D67" s="5"/>
+      <c r="E67" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="K67">
+        <v>1</v>
+      </c>
+      <c r="L67" t="s">
+        <v>219</v>
+      </c>
+      <c r="M67" t="s">
+        <v>220</v>
+      </c>
+      <c r="N67" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>221</v>
       </c>
-      <c r="C67" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E67" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F67" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G67" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="K67">
-        <v>1</v>
-      </c>
-      <c r="L67" t="s">
+      <c r="C68" t="s">
+        <v>14</v>
+      </c>
+      <c r="E68" t="s">
+        <v>8</v>
+      </c>
+      <c r="F68" t="s">
+        <v>15</v>
+      </c>
+      <c r="G68" t="s">
+        <v>212</v>
+      </c>
+      <c r="K68">
+        <v>1</v>
+      </c>
+      <c r="L68" t="s">
         <v>222</v>
       </c>
-      <c r="M67" t="s">
+      <c r="M68" t="s">
         <v>223</v>
       </c>
-      <c r="N67" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A68" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E68" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F68" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G68" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="K68">
-        <v>1</v>
-      </c>
-      <c r="L68" t="s">
-        <v>225</v>
-      </c>
-      <c r="M68" t="s">
-        <v>226</v>
-      </c>
       <c r="N68" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="69" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C69" t="s">
-        <v>19</v>
-      </c>
-      <c r="D69" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E69" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F69" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G69" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K69">
         <v>1</v>
       </c>
       <c r="L69" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="M69" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="N69" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="70" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C70" t="s">
-        <v>19</v>
-      </c>
-      <c r="D70" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E70" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F70" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G70" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K70">
         <v>1</v>
       </c>
       <c r="L70" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="M70" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="N70" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="71" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C71" t="s">
-        <v>19</v>
-      </c>
-      <c r="D71" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E71" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F71" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G71" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K71">
         <v>1</v>
       </c>
       <c r="L71" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="M71" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="N71" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="72" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C72" t="s">
-        <v>19</v>
-      </c>
-      <c r="D72" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E72" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F72" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G72" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K72">
         <v>1</v>
       </c>
       <c r="L72" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="M72" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="N72" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="73" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C73" t="s">
-        <v>19</v>
-      </c>
-      <c r="D73" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E73" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F73" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G73" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K73">
         <v>1</v>
       </c>
       <c r="L73" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="M73" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="N73" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="74" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C74" t="s">
-        <v>19</v>
-      </c>
-      <c r="D74" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E74" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F74" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K74">
         <v>1</v>
       </c>
       <c r="L74" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="M74" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="N74" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="75" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C75" t="s">
-        <v>19</v>
-      </c>
-      <c r="D75" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E75" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F75" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K75">
         <v>1</v>
       </c>
       <c r="L75" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="M75" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="N75" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="76" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C76" t="s">
-        <v>19</v>
-      </c>
-      <c r="D76" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E76" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F76" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G76" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K76">
         <v>1</v>
       </c>
       <c r="L76" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="M76" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="N76" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="77" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C77" t="s">
-        <v>19</v>
-      </c>
-      <c r="D77" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E77" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F77" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G77" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K77">
         <v>1</v>
       </c>
       <c r="L77" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="M77" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="N77" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="78" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C78" t="s">
-        <v>19</v>
-      </c>
-      <c r="D78" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E78" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F78" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K78">
         <v>1</v>
       </c>
       <c r="L78" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="M78" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="N78" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="79" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C79" t="s">
-        <v>19</v>
-      </c>
-      <c r="D79" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E79" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F79" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G79" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K79">
         <v>1</v>
       </c>
       <c r="L79" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="M79" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="N79" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="80" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C80" t="s">
-        <v>19</v>
-      </c>
-      <c r="D80" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E80" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F80" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G80" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K80">
         <v>1</v>
       </c>
       <c r="L80" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="M80" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="N80" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="81" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C81" t="s">
-        <v>19</v>
-      </c>
-      <c r="D81" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E81" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F81" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G81" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K81">
         <v>1</v>
       </c>
       <c r="L81" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="M81" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="N81" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="82" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C82" t="s">
-        <v>19</v>
-      </c>
-      <c r="D82" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E82" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F82" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G82" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K82">
         <v>1</v>
       </c>
       <c r="L82" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="M82" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="N82" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="83" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C83" t="s">
-        <v>19</v>
-      </c>
-      <c r="D83" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E83" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F83" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G83" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K83">
         <v>1</v>
       </c>
       <c r="L83" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="M83" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="N83" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="84" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C84" t="s">
-        <v>19</v>
-      </c>
-      <c r="D84" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E84" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F84" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G84" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K84">
         <v>1</v>
       </c>
       <c r="L84" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="M84" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="N84" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="85" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C85" t="s">
-        <v>19</v>
-      </c>
-      <c r="D85" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E85" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F85" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G85" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K85">
         <v>1</v>
       </c>
       <c r="L85" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="M85" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="N85" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="86" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C86" t="s">
-        <v>19</v>
-      </c>
-      <c r="D86" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E86" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F86" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G86" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K86">
         <v>1</v>
       </c>
       <c r="L86" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="M86" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="N86" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="87" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C87" t="s">
-        <v>19</v>
-      </c>
-      <c r="D87" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E87" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F87" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G87" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K87">
         <v>1</v>
       </c>
       <c r="L87" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="M87" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="N87" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="88" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C88" t="s">
-        <v>19</v>
-      </c>
-      <c r="D88" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E88" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F88" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G88" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K88">
         <v>1</v>
       </c>
       <c r="L88" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="M88" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="N88" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="89" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C89" t="s">
-        <v>19</v>
-      </c>
-      <c r="D89" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E89" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F89" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G89" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K89">
         <v>1</v>
       </c>
       <c r="L89" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="M89" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="N89" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="90" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C90" t="s">
-        <v>19</v>
-      </c>
-      <c r="D90" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E90" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F90" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G90" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K90">
         <v>1</v>
       </c>
       <c r="L90" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="M90" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="N90" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="91" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C91" t="s">
-        <v>19</v>
-      </c>
-      <c r="D91" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E91" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F91" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G91" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K91">
         <v>1</v>
       </c>
       <c r="L91" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="M91" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="N91" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="92" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C92" t="s">
-        <v>19</v>
-      </c>
-      <c r="D92" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E92" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F92" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G92" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K92">
         <v>1</v>
       </c>
       <c r="L92" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="M92" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="N92" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="93" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C93" t="s">
-        <v>19</v>
-      </c>
-      <c r="D93" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E93" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F93" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G93" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K93">
         <v>1</v>
       </c>
       <c r="L93" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="M93" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="N93" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="94" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C94" t="s">
-        <v>19</v>
-      </c>
-      <c r="D94" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E94" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F94" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G94" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K94">
         <v>1</v>
       </c>
       <c r="L94" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="M94" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="N94" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="95" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C95" t="s">
-        <v>19</v>
-      </c>
-      <c r="D95" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E95" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F95" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G95" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K95">
         <v>1</v>
       </c>
       <c r="L95" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="M95" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="N95" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="96" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C96" t="s">
-        <v>19</v>
-      </c>
-      <c r="D96" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E96" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F96" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G96" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K96">
         <v>1</v>
       </c>
       <c r="L96" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="M96" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="N96" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="97" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C97" t="s">
-        <v>19</v>
-      </c>
-      <c r="D97" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E97" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F97" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G97" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K97">
         <v>1</v>
       </c>
       <c r="L97" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="M97" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="N97" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="98" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C98" t="s">
-        <v>19</v>
-      </c>
-      <c r="D98" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E98" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F98" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G98" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K98">
         <v>1</v>
       </c>
       <c r="L98" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="M98" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="N98" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="99" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C99" t="s">
-        <v>19</v>
-      </c>
-      <c r="D99" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E99" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F99" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G99" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K99">
         <v>1</v>
       </c>
       <c r="L99" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="M99" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="N99" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="100" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C100" t="s">
-        <v>19</v>
-      </c>
-      <c r="D100" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E100" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F100" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G100" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K100">
         <v>1</v>
       </c>
       <c r="L100" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="M100" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="N100" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="101" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C101" t="s">
-        <v>19</v>
-      </c>
-      <c r="D101" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E101" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F101" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G101" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K101">
         <v>1</v>
       </c>
       <c r="L101" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="M101" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="N101" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="102" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C102" t="s">
-        <v>19</v>
-      </c>
-      <c r="D102" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E102" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F102" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G102" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K102">
         <v>1</v>
       </c>
       <c r="L102" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="M102" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="N102" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="103" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C103" t="s">
-        <v>19</v>
-      </c>
-      <c r="D103" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E103" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F103" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G103" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K103">
         <v>1</v>
       </c>
       <c r="L103" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="M103" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="N103" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="104" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C104" t="s">
-        <v>19</v>
-      </c>
-      <c r="D104" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E104" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F104" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G104" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K104">
         <v>1</v>
       </c>
       <c r="L104" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="M104" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="N104" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="105" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>335</v>
-      </c>
-      <c r="C105" t="s">
-        <v>19</v>
-      </c>
-      <c r="D105" t="s">
-        <v>20</v>
-      </c>
-      <c r="E105" t="s">
-        <v>11</v>
-      </c>
-      <c r="F105" t="s">
-        <v>21</v>
-      </c>
-      <c r="G105" t="s">
-        <v>218</v>
-      </c>
-      <c r="K105">
-        <v>1</v>
-      </c>
-      <c r="L105" t="s">
-        <v>336</v>
-      </c>
-      <c r="M105" t="s">
-        <v>337</v>
-      </c>
-      <c r="N105" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>